<commit_message>
modelim can be sent
</commit_message>
<xml_diff>
--- a/lbl/Progress.xlsx
+++ b/lbl/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\!Summaries\lbl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61802C66-3E5D-47B9-92B2-34DCABC9722C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7692290-D525-4919-8769-0DB1AED1A08F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -403,7 +403,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,7 +462,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>45488</v>
+        <v>45495</v>
       </c>
       <c r="D4">
         <v>0</v>

</xml_diff>

<commit_message>
Commit - 10/09/2024 21:37:09
</commit_message>
<xml_diff>
--- a/lbl/Progress.xlsx
+++ b/lbl/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\!Summaries\lbl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250B5800-C80F-44A4-BD61-962CF5BFE260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F232962C-10F6-40D6-AF7C-3365621FB5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -416,7 +416,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,14 +481,9 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
-        <v>45502</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <v>9</v>
+      <c r="B4" s="1"/>
+      <c r="C4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Commit - 10/09/2024 21:38:23
</commit_message>
<xml_diff>
--- a/lbl/Progress.xlsx
+++ b/lbl/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\!Summaries\lbl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F232962C-10F6-40D6-AF7C-3365621FB5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B906082B-B666-4112-A80E-89CC576FBD66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Need formatting</t>
+  </si>
+  <si>
+    <t>Complete gedels proof</t>
   </si>
 </sst>
 </file>
@@ -416,7 +419,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,14 +470,12 @@
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1">
-        <v>45501</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
+      <c r="B3" s="1"/>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Commit - 17/09/2024 02:44:54
</commit_message>
<xml_diff>
--- a/lbl/Progress.xlsx
+++ b/lbl/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\!Summaries\lbl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B906082B-B666-4112-A80E-89CC576FBD66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2021A6-4C92-4072-BE6A-032EA3408A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,10 +72,10 @@
     <t>Need algorithms in the end</t>
   </si>
   <si>
-    <t>Need formatting</t>
-  </si>
-  <si>
-    <t>Complete gedels proof</t>
+    <t>Add algorithms, Complete gedels proof</t>
+  </si>
+  <si>
+    <t>ode</t>
   </si>
 </sst>
 </file>
@@ -136,10 +136,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{038D390C-8F1B-4F12-84BC-66648BC6E07A}" name="Table1" displayName="Table1" ref="A1:F7">
-  <autoFilter ref="A1:F7" xr:uid="{038D390C-8F1B-4F12-84BC-66648BC6E07A}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F7">
-    <sortCondition ref="B1:B7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{038D390C-8F1B-4F12-84BC-66648BC6E07A}" name="Table1" displayName="Table1" ref="A1:F8">
+  <autoFilter ref="A1:F8" xr:uid="{038D390C-8F1B-4F12-84BC-66648BC6E07A}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F8">
+    <sortCondition ref="B1:B8"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{A14A81E1-C0C7-49D1-9D52-9F18C7DCCFDD}" name="Name" totalsRowLabel="Total"/>
@@ -416,7 +416,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
@@ -451,72 +451,78 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1">
-        <v>45489</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
+        <v>45438</v>
+      </c>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
+        <v>5</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45489</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" t="s">
         <v>13</v>
       </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" t="s">
         <v>13</v>
       </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" t="s">
         <v>13</v>
       </c>
-      <c r="F7" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>